<commit_message>
Atualização de algun pesos
</commit_message>
<xml_diff>
--- a/Producao/Combate_1kg/Pesos atualizados.xlsx
+++ b/Producao/Combate_1kg/Pesos atualizados.xlsx
@@ -11,13 +11,78 @@
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>Peso(g)</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Lateral (Al)</t>
+  </si>
+  <si>
+    <t>Cobertura (A definir)</t>
+  </si>
+  <si>
+    <t>Chassi (PETG)</t>
+  </si>
+  <si>
+    <t>motor arma</t>
+  </si>
+  <si>
+    <t>bateria</t>
+  </si>
+  <si>
+    <t>receptor</t>
+  </si>
+  <si>
+    <t>ESC</t>
+  </si>
+  <si>
+    <t>Suporte motor mov(Al)</t>
+  </si>
+  <si>
+    <t>Arma (Aço + Al)</t>
+  </si>
+  <si>
+    <t>Rolamentos</t>
+  </si>
+  <si>
+    <t>Correia + Polias</t>
+  </si>
+  <si>
+    <t>Placa de controle</t>
+  </si>
+  <si>
+    <t>motores mov</t>
+  </si>
+  <si>
+    <t>Fios + conectores</t>
+  </si>
+  <si>
+    <t>Parafusos</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Rodas</t>
+  </si>
+  <si>
+    <t>Mancal  arma (Pol)</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,19 +90,58 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -46,8 +150,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,12 +453,172 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3">
+        <f>SUM(B2:B18)</f>
+        <v>1550</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>

<commit_message>
atualização do layout da placa
</commit_message>
<xml_diff>
--- a/Producao/Combate_1kg/Pesos atualizados.xlsx
+++ b/Producao/Combate_1kg/Pesos atualizados.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Peso(g)</t>
   </si>
@@ -30,15 +30,9 @@
     <t>Cobertura (A definir)</t>
   </si>
   <si>
-    <t>Chassi (PETG)</t>
-  </si>
-  <si>
     <t>motor arma</t>
   </si>
   <si>
-    <t>bateria</t>
-  </si>
-  <si>
     <t>receptor</t>
   </si>
   <si>
@@ -66,9 +60,6 @@
     <t>Fios + conectores</t>
   </si>
   <si>
-    <t>Parafusos</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
@@ -76,13 +67,37 @@
   </si>
   <si>
     <t>Mancal  arma (Pol)</t>
+  </si>
+  <si>
+    <t>5 cada</t>
+  </si>
+  <si>
+    <t>Eixo</t>
+  </si>
+  <si>
+    <t>Detalhes</t>
+  </si>
+  <si>
+    <t>Bits</t>
+  </si>
+  <si>
+    <t>Discos</t>
+  </si>
+  <si>
+    <t>Chassi (PETG) 50% treliça</t>
+  </si>
+  <si>
+    <t>bateria (2S 1700mAh)</t>
+  </si>
+  <si>
+    <t>Parafusos (Reduzidos)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +108,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -150,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -159,6 +180,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -465,7 +490,7 @@
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -473,15 +498,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="B2" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -489,113 +514,138 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="E6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
+        <f>SUM(E7:G7)</f>
+        <v>317</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="7">
+        <v>47</v>
+      </c>
+      <c r="F7" s="7">
+        <v>102</v>
+      </c>
+      <c r="G7" s="7">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="6">
         <v>10</v>
       </c>
-      <c r="B7" s="2">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="5" t="s">
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="6">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B9" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="B10" s="2">
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B12" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="B14" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B15" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" s="2">
         <v>50</v>
@@ -603,24 +653,24 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B18" s="2">
-        <v>120</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B19" s="3">
         <f>SUM(B2:B18)</f>
-        <v>1550</v>
+        <v>1470</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>